<commit_message>
Completed test summary for best effort multicast
</commit_message>
<xml_diff>
--- a/Tests/Set 14 [Set 13 Best Effort Rerun]/Best Effort Multicast/Best Effort Multicast Test Summary.xlsx
+++ b/Tests/Set 14 [Set 13 Best Effort Rerun]/Best Effort Multicast/Best Effort Multicast Test Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalee\Documents\Performance-Testing\Tests\Set 14 [Set 13 Best Effort Rerun]\Best Effort Multicast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaleem/Documents/performance-testing/Tests/Set 14 [Set 13 Best Effort Rerun]/Best Effort Multicast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFF7BAF-FC44-494A-A48B-52DFAFE90E70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C247B4-3728-574B-8808-91B2B53A037A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Config" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -864,29 +864,29 @@
   <dimension ref="B2:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:H14"/>
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5" style="14" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="14"/>
+    <col min="13" max="16384" width="9.1640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="28">
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="16">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -897,7 +897,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="16">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="16">
       <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
@@ -927,7 +927,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="16">
       <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
@@ -942,7 +942,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="16">
       <c r="B8" s="13"/>
       <c r="C8" s="4"/>
       <c r="D8" s="7"/>
@@ -953,12 +953,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="19">
       <c r="B10" s="28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12">
       <c r="B11" s="18"/>
       <c r="C11" s="19" t="s">
         <v>18</v>
@@ -979,40 +979,76 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="22">
+        <v>51</v>
+      </c>
+      <c r="D12" s="16">
+        <v>66275542</v>
+      </c>
+      <c r="E12" s="16">
+        <v>33724457</v>
+      </c>
+      <c r="F12" s="16">
+        <v>809</v>
+      </c>
+      <c r="G12" s="23">
+        <v>1739</v>
+      </c>
+      <c r="H12" s="23">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="20">
+        <v>49</v>
+      </c>
+      <c r="D13" s="20">
+        <v>61918310</v>
+      </c>
+      <c r="E13" s="20">
+        <v>38076628</v>
+      </c>
+      <c r="F13" s="20">
+        <v>920</v>
+      </c>
+      <c r="G13" s="24">
+        <v>1762</v>
+      </c>
+      <c r="H13" s="24">
+        <v>2822</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
       <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="17">
+        <v>55</v>
+      </c>
+      <c r="D14" s="17">
+        <v>73724705</v>
+      </c>
+      <c r="E14" s="17">
+        <v>26196677</v>
+      </c>
+      <c r="F14" s="17">
+        <v>984</v>
+      </c>
+      <c r="G14" s="25">
+        <v>3317</v>
+      </c>
+      <c r="H14" s="25">
+        <v>4481</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
@@ -1025,7 +1061,7 @@
       <c r="K15" s="26"/>
       <c r="L15" s="26"/>
     </row>
-    <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="19">
       <c r="B16" s="29" t="s">
         <v>19</v>
       </c>
@@ -1040,7 +1076,7 @@
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12">
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
@@ -1053,7 +1089,7 @@
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="C18" s="21" t="s">
         <v>27</v>
       </c>
@@ -1069,36 +1105,54 @@
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="49"/>
+      <c r="C19" s="50">
+        <v>3201</v>
+      </c>
+      <c r="D19" s="51">
+        <v>6936</v>
+      </c>
+      <c r="E19" s="49">
+        <v>968</v>
+      </c>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="54"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C20" s="52">
+        <v>3363</v>
+      </c>
+      <c r="D20" s="53">
+        <v>6339</v>
+      </c>
+      <c r="E20" s="54">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
       <c r="B21" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C21" s="55">
+        <v>4252</v>
+      </c>
+      <c r="D21" s="56">
+        <v>7507</v>
+      </c>
+      <c r="E21" s="57">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
       <c r="C23" s="31"/>
       <c r="D23" s="32"/>
       <c r="E23" s="32" t="s">
@@ -1107,7 +1161,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12">
       <c r="C24" s="40" t="s">
         <v>34</v>
       </c>
@@ -1124,37 +1178,67 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12">
       <c r="B25" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C25" s="31">
+        <v>30</v>
+      </c>
+      <c r="D25" s="32">
+        <v>30</v>
+      </c>
+      <c r="E25" s="32">
+        <v>30</v>
+      </c>
+      <c r="F25" s="32">
+        <v>30</v>
+      </c>
+      <c r="G25" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
       <c r="B26" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="60"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C26" s="58">
+        <v>32</v>
+      </c>
+      <c r="D26" s="59">
+        <v>32</v>
+      </c>
+      <c r="E26" s="59">
+        <v>31</v>
+      </c>
+      <c r="F26" s="59">
+        <v>31</v>
+      </c>
+      <c r="G26" s="60">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
       <c r="B27" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="34"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C27" s="34">
+        <v>34</v>
+      </c>
+      <c r="D27" s="35">
+        <v>34</v>
+      </c>
+      <c r="E27" s="35">
+        <v>32</v>
+      </c>
+      <c r="F27" s="35">
+        <v>32</v>
+      </c>
+      <c r="G27" s="36">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
       <c r="C29" s="37"/>
       <c r="D29" s="38"/>
       <c r="E29" s="38" t="s">
@@ -1163,7 +1247,7 @@
       <c r="F29" s="38"/>
       <c r="G29" s="39"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12">
       <c r="C30" s="40" t="s">
         <v>34</v>
       </c>
@@ -1180,37 +1264,67 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12">
       <c r="B31" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C31" s="31">
+        <v>39500911</v>
+      </c>
+      <c r="D31" s="32">
+        <v>39504824</v>
+      </c>
+      <c r="E31" s="32">
+        <v>40296194</v>
+      </c>
+      <c r="F31" s="32">
+        <v>40288859</v>
+      </c>
+      <c r="G31" s="33">
+        <v>73477930</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12">
       <c r="B32" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="60"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="58">
+        <v>44795490</v>
+      </c>
+      <c r="D32" s="59">
+        <v>44789117</v>
+      </c>
+      <c r="E32" s="59">
+        <v>43980234</v>
+      </c>
+      <c r="F32" s="59">
+        <v>43974826</v>
+      </c>
+      <c r="G32" s="60">
+        <v>79970422</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
       <c r="B33" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="34">
+        <v>48681368</v>
+      </c>
+      <c r="D33" s="35">
+        <v>48724360</v>
+      </c>
+      <c r="E33" s="35">
+        <v>46723542</v>
+      </c>
+      <c r="F33" s="35">
+        <v>46822499</v>
+      </c>
+      <c r="G33" s="35">
+        <v>78796462</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
       <c r="C35" s="37"/>
       <c r="D35" s="38"/>
       <c r="E35" s="38" t="s">
@@ -1219,7 +1333,7 @@
       <c r="F35" s="38"/>
       <c r="G35" s="39"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7">
       <c r="C36" s="40" t="s">
         <v>34</v>
       </c>
@@ -1236,37 +1350,67 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7">
       <c r="B37" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="31">
+        <v>60465361</v>
+      </c>
+      <c r="D37" s="32">
+        <v>60429029</v>
+      </c>
+      <c r="E37" s="32">
+        <v>59703806</v>
+      </c>
+      <c r="F37" s="32">
+        <v>59711141</v>
+      </c>
+      <c r="G37" s="33">
+        <v>26430944</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
       <c r="B38" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="60"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="58">
+        <v>55204510</v>
+      </c>
+      <c r="D38" s="59">
+        <v>55210883</v>
+      </c>
+      <c r="E38" s="59">
+        <v>55935594</v>
+      </c>
+      <c r="F38" s="59">
+        <v>55941002</v>
+      </c>
+      <c r="G38" s="60">
+        <v>20000350</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
       <c r="B39" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="36"/>
-    </row>
-    <row r="42" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C39" s="34">
+        <v>51247387</v>
+      </c>
+      <c r="D39" s="35">
+        <v>51204395</v>
+      </c>
+      <c r="E39" s="35">
+        <v>53231255</v>
+      </c>
+      <c r="F39" s="35">
+        <v>53132298</v>
+      </c>
+      <c r="G39" s="35">
+        <v>21175897</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="19">
       <c r="B42" s="29" t="s">
         <v>29</v>
       </c>
@@ -1275,14 +1419,14 @@
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7">
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7">
       <c r="C44" s="21" t="s">
         <v>27</v>
       </c>
@@ -1293,31 +1437,49 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7">
       <c r="B45" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="49"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="50">
+        <v>3149</v>
+      </c>
+      <c r="D45" s="51">
+        <v>11761</v>
+      </c>
+      <c r="E45" s="49">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
       <c r="B46" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="52"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="54"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="52">
+        <v>3213</v>
+      </c>
+      <c r="D46" s="53">
+        <v>11245</v>
+      </c>
+      <c r="E46" s="54">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
       <c r="B47" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="57"/>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C47" s="55">
+        <v>4252</v>
+      </c>
+      <c r="D47" s="56">
+        <v>7507</v>
+      </c>
+      <c r="E47" s="57">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12">
       <c r="C49" s="31"/>
       <c r="D49" s="32"/>
       <c r="E49" s="32"/>
@@ -1331,7 +1493,7 @@
       <c r="K49" s="32"/>
       <c r="L49" s="33"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12">
       <c r="C50" s="40" t="s">
         <v>34</v>
       </c>
@@ -1363,52 +1525,112 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12">
       <c r="B51" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="44"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C51" s="42">
+        <v>22</v>
+      </c>
+      <c r="D51" s="43">
+        <v>22</v>
+      </c>
+      <c r="E51" s="43">
+        <v>22</v>
+      </c>
+      <c r="F51" s="43">
+        <v>23</v>
+      </c>
+      <c r="G51" s="32">
+        <v>23</v>
+      </c>
+      <c r="H51" s="43">
+        <v>23</v>
+      </c>
+      <c r="I51" s="43">
+        <v>15</v>
+      </c>
+      <c r="J51" s="43">
+        <v>15</v>
+      </c>
+      <c r="K51" s="43">
+        <v>15</v>
+      </c>
+      <c r="L51" s="44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12">
       <c r="B52" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C52" s="58"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="59"/>
-      <c r="J52" s="59"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="60"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C52" s="58">
+        <v>22</v>
+      </c>
+      <c r="D52" s="59">
+        <v>22</v>
+      </c>
+      <c r="E52" s="59">
+        <v>22</v>
+      </c>
+      <c r="F52" s="59">
+        <v>20</v>
+      </c>
+      <c r="G52" s="59">
+        <v>20</v>
+      </c>
+      <c r="H52" s="59">
+        <v>20</v>
+      </c>
+      <c r="I52" s="59">
+        <v>15</v>
+      </c>
+      <c r="J52" s="59">
+        <v>15</v>
+      </c>
+      <c r="K52" s="59">
+        <v>15</v>
+      </c>
+      <c r="L52" s="60">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12">
       <c r="B53" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="34"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="36"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C53" s="34">
+        <v>21</v>
+      </c>
+      <c r="D53" s="35">
+        <v>21</v>
+      </c>
+      <c r="E53" s="35">
+        <v>21</v>
+      </c>
+      <c r="F53" s="35">
+        <v>20</v>
+      </c>
+      <c r="G53" s="35">
+        <v>20</v>
+      </c>
+      <c r="H53" s="35">
+        <v>20</v>
+      </c>
+      <c r="I53" s="35">
+        <v>16</v>
+      </c>
+      <c r="J53" s="35">
+        <v>16</v>
+      </c>
+      <c r="K53" s="35">
+        <v>16</v>
+      </c>
+      <c r="L53" s="36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12">
       <c r="C55" s="37"/>
       <c r="D55" s="38"/>
       <c r="E55" s="38"/>
@@ -1422,7 +1644,7 @@
       <c r="K55" s="32"/>
       <c r="L55" s="33"/>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12">
       <c r="C56" s="40" t="s">
         <v>34</v>
       </c>
@@ -1454,52 +1676,112 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12">
       <c r="B57" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="42"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="43"/>
-      <c r="K57" s="43"/>
-      <c r="L57" s="44"/>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C57" s="42">
+        <v>29056198</v>
+      </c>
+      <c r="D57" s="43">
+        <v>29061733</v>
+      </c>
+      <c r="E57" s="43">
+        <v>29026758</v>
+      </c>
+      <c r="F57" s="43">
+        <v>29659950</v>
+      </c>
+      <c r="G57" s="32">
+        <v>29645723</v>
+      </c>
+      <c r="H57" s="43">
+        <v>29645123</v>
+      </c>
+      <c r="I57" s="43">
+        <v>19152994</v>
+      </c>
+      <c r="J57" s="43">
+        <v>19128708</v>
+      </c>
+      <c r="K57" s="43">
+        <v>19125895</v>
+      </c>
+      <c r="L57" s="44">
+        <v>19114603</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12">
       <c r="B58" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C58" s="58"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="59"/>
-      <c r="G58" s="59"/>
-      <c r="H58" s="59"/>
-      <c r="I58" s="59"/>
-      <c r="J58" s="59"/>
-      <c r="K58" s="59"/>
-      <c r="L58" s="60"/>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C58" s="58">
+        <v>31231341</v>
+      </c>
+      <c r="D58" s="59">
+        <v>31237644</v>
+      </c>
+      <c r="E58" s="59">
+        <v>31216018</v>
+      </c>
+      <c r="F58" s="59">
+        <v>28721135</v>
+      </c>
+      <c r="G58" s="59">
+        <v>28295847</v>
+      </c>
+      <c r="H58" s="59">
+        <v>28309343</v>
+      </c>
+      <c r="I58" s="59">
+        <v>21429032</v>
+      </c>
+      <c r="J58" s="59">
+        <v>21429032</v>
+      </c>
+      <c r="K58" s="59">
+        <v>21429032</v>
+      </c>
+      <c r="L58" s="60">
+        <v>21422162</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12">
       <c r="B59" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="34"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="36"/>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C59" s="34">
+        <v>28891566</v>
+      </c>
+      <c r="D59" s="35">
+        <v>28889266</v>
+      </c>
+      <c r="E59" s="35">
+        <v>28901717</v>
+      </c>
+      <c r="F59" s="35">
+        <v>27392614</v>
+      </c>
+      <c r="G59" s="36">
+        <v>27392356</v>
+      </c>
+      <c r="H59" s="35">
+        <v>27400767</v>
+      </c>
+      <c r="I59" s="35">
+        <v>21230891</v>
+      </c>
+      <c r="J59" s="35">
+        <v>21230891</v>
+      </c>
+      <c r="K59" s="35">
+        <v>21230891</v>
+      </c>
+      <c r="L59" s="35">
+        <v>21230891</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12">
       <c r="C61" s="37"/>
       <c r="D61" s="38"/>
       <c r="E61" s="38"/>
@@ -1513,7 +1795,7 @@
       <c r="K61" s="32"/>
       <c r="L61" s="33"/>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12">
       <c r="C62" s="40" t="s">
         <v>34</v>
       </c>
@@ -1545,50 +1827,110 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12">
       <c r="B63" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="32"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="43"/>
-      <c r="K63" s="43"/>
-      <c r="L63" s="44"/>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C63" s="31">
+        <v>70943802</v>
+      </c>
+      <c r="D63" s="32">
+        <v>70938267</v>
+      </c>
+      <c r="E63" s="32">
+        <v>70835662</v>
+      </c>
+      <c r="F63" s="32">
+        <v>70329343</v>
+      </c>
+      <c r="G63" s="32">
+        <v>70343570</v>
+      </c>
+      <c r="H63" s="43">
+        <v>70344170</v>
+      </c>
+      <c r="I63" s="43">
+        <v>80793872</v>
+      </c>
+      <c r="J63" s="43">
+        <v>80818518</v>
+      </c>
+      <c r="K63" s="43">
+        <v>80820971</v>
+      </c>
+      <c r="L63" s="44">
+        <v>80832263</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12">
       <c r="B64" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="58"/>
-      <c r="D64" s="59"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="59"/>
-      <c r="G64" s="59"/>
-      <c r="H64" s="59"/>
-      <c r="I64" s="59"/>
-      <c r="J64" s="59"/>
-      <c r="K64" s="59"/>
-      <c r="L64" s="60"/>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C64" s="58">
+        <v>68727073</v>
+      </c>
+      <c r="D64" s="59">
+        <v>68720770</v>
+      </c>
+      <c r="E64" s="59">
+        <v>68742396</v>
+      </c>
+      <c r="F64" s="59">
+        <v>71275662</v>
+      </c>
+      <c r="G64" s="59">
+        <v>71700950</v>
+      </c>
+      <c r="H64" s="59">
+        <v>71687454</v>
+      </c>
+      <c r="I64" s="59">
+        <v>78527265</v>
+      </c>
+      <c r="J64" s="59">
+        <v>78527265</v>
+      </c>
+      <c r="K64" s="59">
+        <v>78527265</v>
+      </c>
+      <c r="L64" s="60">
+        <v>78534135</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12">
       <c r="B65" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="34"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="35"/>
-      <c r="K65" s="35"/>
-      <c r="L65" s="36"/>
+      <c r="C65" s="34">
+        <v>71096707</v>
+      </c>
+      <c r="D65" s="35">
+        <v>71099007</v>
+      </c>
+      <c r="E65" s="35">
+        <v>71086556</v>
+      </c>
+      <c r="F65" s="35">
+        <v>72588989</v>
+      </c>
+      <c r="G65" s="36">
+        <v>72589247</v>
+      </c>
+      <c r="H65" s="35">
+        <v>72580836</v>
+      </c>
+      <c r="I65" s="35">
+        <v>78741131</v>
+      </c>
+      <c r="J65" s="35">
+        <v>78741131</v>
+      </c>
+      <c r="K65" s="35">
+        <v>78741131</v>
+      </c>
+      <c r="L65" s="35">
+        <v>78741131</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1602,7 +1944,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>